<commit_message>
Commit he thong - Huy
</commit_message>
<xml_diff>
--- a/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
+++ b/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HuyNguyen\Desktop\VatLieuXayDung\QuanLyCuaHangVLXD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kiểm thử\New folder\QuanLyCuaHangVLXD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
   <si>
     <t>1.    Phạm vi test</t>
   </si>
@@ -479,6 +479,9 @@
   <si>
     <t>- Hiển thị thông báo "Bạn phải nhập mã khách hàng cần tìm kiếm"
 - Tìm kiếm thất bại.</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
@@ -987,50 +990,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1042,7 +1045,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="89">
+  <dxfs count="92">
     <dxf>
       <fill>
         <patternFill>
@@ -1194,6 +1197,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2093,7 +2117,7 @@
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
+      <c r="E1" s="59"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -2102,47 +2126,47 @@
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="54" t="s">
+      <c r="I2" s="52"/>
+      <c r="J2" s="53" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="55"/>
+      <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
@@ -2193,7 +2217,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="44"/>
-      <c r="C7" s="48"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="5"/>
@@ -2208,8 +2232,8 @@
       <c r="C8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="15"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -2222,8 +2246,8 @@
       <c r="C9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="15"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -2236,8 +2260,8 @@
       <c r="C10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
       <c r="F10" s="15"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -2269,11 +2293,11 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -2296,6 +2320,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="G2:G3"/>
@@ -2305,11 +2334,6 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -2320,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2421,7 +2445,9 @@
         <v>38</v>
       </c>
       <c r="J3" s="20"/>
-      <c r="K3" s="24"/>
+      <c r="K3" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L3" s="19"/>
       <c r="V3" s="21"/>
     </row>
@@ -4084,303 +4110,316 @@
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K1:K17 K19:K20">
-    <cfRule type="containsText" dxfId="88" priority="84" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K1:K2 K19:K20 K4:K17">
+    <cfRule type="containsText" dxfId="91" priority="87" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K17 K19:K20">
-    <cfRule type="containsText" dxfId="87" priority="82" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K4:K17 K19:K20">
+    <cfRule type="containsText" dxfId="90" priority="85" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="86" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="containsText" dxfId="88" priority="81" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="containsText" dxfId="87" priority="79" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="86" priority="80" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="containsText" dxfId="85" priority="78" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="containsText" dxfId="84" priority="76" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="83" priority="77" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23:K29">
+    <cfRule type="containsText" dxfId="82" priority="75" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23:K29">
+    <cfRule type="containsText" dxfId="81" priority="73" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="74" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30">
+    <cfRule type="containsText" dxfId="79" priority="72" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30">
+    <cfRule type="containsText" dxfId="78" priority="70" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="71" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="containsText" dxfId="76" priority="69" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="containsText" dxfId="75" priority="67" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="68" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32">
+    <cfRule type="containsText" dxfId="73" priority="66" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32">
+    <cfRule type="containsText" dxfId="72" priority="64" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="71" priority="65" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33:K45">
+    <cfRule type="containsText" dxfId="70" priority="63" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33:K45">
+    <cfRule type="containsText" dxfId="69" priority="61" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="62" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46">
+    <cfRule type="containsText" dxfId="67" priority="60" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46">
+    <cfRule type="containsText" dxfId="66" priority="58" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="59" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="containsText" dxfId="63" priority="55" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="56" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="containsText" dxfId="60" priority="52" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K55">
+    <cfRule type="containsText" dxfId="58" priority="51" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K55">
+    <cfRule type="containsText" dxfId="57" priority="49" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="50" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:K61">
+    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:K61">
+    <cfRule type="containsText" dxfId="54" priority="34" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="35" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="29" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65:K71">
+    <cfRule type="containsText" dxfId="43" priority="24" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65:K71">
+    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:K79">
+    <cfRule type="containsText" dxfId="40" priority="21" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:K79">
+    <cfRule type="containsText" dxfId="39" priority="19" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K72)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="20" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80">
+    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80">
+    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K80)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="17" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81">
+    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K81)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82">
+    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82">
+    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K82)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K83:K89">
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K83:K89">
+    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K83)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="83" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="85" priority="78" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="84" priority="76" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="77" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
-    <cfRule type="containsText" dxfId="82" priority="75" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
-    <cfRule type="containsText" dxfId="81" priority="73" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="74" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23:K29">
-    <cfRule type="containsText" dxfId="79" priority="72" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23:K29">
-    <cfRule type="containsText" dxfId="78" priority="70" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="71" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="76" priority="69" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="75" priority="67" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="68" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="73" priority="66" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="72" priority="64" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="65" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="70" priority="63" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="69" priority="61" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="62" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K33:K45">
-    <cfRule type="containsText" dxfId="67" priority="60" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K33:K45">
-    <cfRule type="containsText" dxfId="66" priority="58" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="59" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="63" priority="55" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="56" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47">
-    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47">
-    <cfRule type="containsText" dxfId="60" priority="52" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K48">
-    <cfRule type="containsText" dxfId="58" priority="51" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K48">
-    <cfRule type="containsText" dxfId="57" priority="49" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="50" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K49:K55">
-    <cfRule type="containsText" dxfId="55" priority="48" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K49:K55">
-    <cfRule type="containsText" dxfId="54" priority="46" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="47" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K56:K61">
-    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K56:K61">
-    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K62)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="29" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="43" priority="24" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65:K71">
-    <cfRule type="containsText" dxfId="40" priority="21" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65:K71">
-    <cfRule type="containsText" dxfId="39" priority="19" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="20" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72:K79">
-    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72:K79">
-    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K72)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="17" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K80">
-    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K80)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K80">
-    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K80)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K80)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81">
-    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81">
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K81)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82">
-    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82">
-    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K82)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K83:K89">
-    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K83)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K83:K89">
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K83)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K83)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Them CSDL cap nhat moi
</commit_message>
<xml_diff>
--- a/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
+++ b/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="117">
   <si>
     <t>1.    Phạm vi test</t>
   </si>
@@ -1045,7 +1045,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="95">
     <dxf>
       <fill>
         <patternFill>
@@ -1078,6 +1078,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2345,7 +2366,7 @@
   <dimension ref="A1:V89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2478,7 +2499,9 @@
         <v>38</v>
       </c>
       <c r="J4" s="20"/>
-      <c r="K4" s="24"/>
+      <c r="K4" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L4" s="19"/>
     </row>
     <row r="5" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -4110,316 +4133,329 @@
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K1:K2 K19:K20 K4:K17">
-    <cfRule type="containsText" dxfId="91" priority="87" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K1:K2 K19:K20 K5:K17">
+    <cfRule type="containsText" dxfId="94" priority="90" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K17 K19:K20">
-    <cfRule type="containsText" dxfId="90" priority="85" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K5:K17 K19:K20">
+    <cfRule type="containsText" dxfId="93" priority="88" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="89" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="containsText" dxfId="91" priority="84" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="containsText" dxfId="90" priority="82" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="83" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="containsText" dxfId="88" priority="81" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="containsText" dxfId="87" priority="79" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="86" priority="80" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23:K29">
+    <cfRule type="containsText" dxfId="85" priority="78" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23:K29">
+    <cfRule type="containsText" dxfId="84" priority="76" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="83" priority="77" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30">
+    <cfRule type="containsText" dxfId="82" priority="75" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30">
+    <cfRule type="containsText" dxfId="81" priority="73" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="74" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="containsText" dxfId="79" priority="72" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="containsText" dxfId="78" priority="70" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="71" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32">
+    <cfRule type="containsText" dxfId="76" priority="69" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32">
+    <cfRule type="containsText" dxfId="75" priority="67" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="68" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33:K45">
+    <cfRule type="containsText" dxfId="73" priority="66" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33:K45">
+    <cfRule type="containsText" dxfId="72" priority="64" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="71" priority="65" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46">
+    <cfRule type="containsText" dxfId="70" priority="63" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46">
+    <cfRule type="containsText" dxfId="69" priority="61" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="62" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="containsText" dxfId="67" priority="60" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="containsText" dxfId="66" priority="58" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="59" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="containsText" dxfId="63" priority="55" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="56" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K55">
+    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K55">
+    <cfRule type="containsText" dxfId="60" priority="52" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:K61">
+    <cfRule type="containsText" dxfId="58" priority="39" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:K61">
+    <cfRule type="containsText" dxfId="57" priority="37" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="38" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="containsText" dxfId="54" priority="34" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="35" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="29" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65:K71">
+    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65:K71">
+    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:K79">
+    <cfRule type="containsText" dxfId="43" priority="24" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:K79">
+    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K72)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80">
+    <cfRule type="containsText" dxfId="40" priority="21" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80">
+    <cfRule type="containsText" dxfId="39" priority="19" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K80)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="20" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81">
+    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81">
+    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K81)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="17" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82">
+    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K82)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K83:K89">
+    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K83:K89">
+    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K83)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="86" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="88" priority="81" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="87" priority="79" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="80" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
-    <cfRule type="containsText" dxfId="85" priority="78" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
-    <cfRule type="containsText" dxfId="84" priority="76" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="77" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23:K29">
-    <cfRule type="containsText" dxfId="82" priority="75" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23:K29">
-    <cfRule type="containsText" dxfId="81" priority="73" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="74" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="79" priority="72" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="78" priority="70" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="71" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="76" priority="69" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="75" priority="67" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="68" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="73" priority="66" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="72" priority="64" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="65" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K33:K45">
-    <cfRule type="containsText" dxfId="70" priority="63" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K33:K45">
-    <cfRule type="containsText" dxfId="69" priority="61" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="62" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="67" priority="60" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="66" priority="58" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="59" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47">
-    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47">
-    <cfRule type="containsText" dxfId="63" priority="55" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="56" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K48">
-    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K48">
-    <cfRule type="containsText" dxfId="60" priority="52" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K49:K55">
-    <cfRule type="containsText" dxfId="58" priority="51" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K49:K55">
-    <cfRule type="containsText" dxfId="57" priority="49" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="50" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K56:K61">
-    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K56:K61">
-    <cfRule type="containsText" dxfId="54" priority="34" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="35" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K62)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="29" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65:K71">
-    <cfRule type="containsText" dxfId="43" priority="24" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65:K71">
-    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72:K79">
-    <cfRule type="containsText" dxfId="40" priority="21" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72:K79">
-    <cfRule type="containsText" dxfId="39" priority="19" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K72)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="20" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K80">
-    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K80)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K80">
-    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K80)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="17" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K80)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81">
-    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81">
-    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K81)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82">
-    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82">
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K82)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K83:K89">
-    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K83)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K83:K89">
-    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K83)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K83)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -4589,77 +4625,77 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="L1">
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="23" priority="15" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="22" priority="13" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="20" priority="12" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="containsText" dxfId="16" priority="10" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="19" priority="10" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="16" priority="7" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L7)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Test Case Form Dat hang
</commit_message>
<xml_diff>
--- a/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
+++ b/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="174">
   <si>
     <t>1.    Phạm vi test</t>
   </si>
@@ -483,12 +483,249 @@
   <si>
     <t>Passed</t>
   </si>
+  <si>
+    <t>SCM-20</t>
+  </si>
+  <si>
+    <t>SCM-22</t>
+  </si>
+  <si>
+    <t>Đặt hàng</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Hệ thống chưa xử lý được</t>
+  </si>
+  <si>
+    <t>Chọn ngày giao hàng trước ngày đặt hàng</t>
+  </si>
+  <si>
+    <t>1. Chọn ngày giao hàng trước ngày đặt hàng</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "Phải chọn ngày giao hàng sau ngày đặt hàng"
+- Không thể đặt hàng</t>
+  </si>
+  <si>
+    <t>SCM-21</t>
+  </si>
+  <si>
+    <t>Chọn ngày giao hàng cùng ngày với ngày đặt hàng</t>
+  </si>
+  <si>
+    <t>1. Chọn ngày giao hàng cùng ngày với ngày đặt hàng</t>
+  </si>
+  <si>
+    <t>Chọn ngày giao hàng sau ngày đặt hàng</t>
+  </si>
+  <si>
+    <t>1. Chọn ngày giao hàng sau ngày đặt hàng
+2. Bấm nút "Thêm"
+2. Xác nhận Tạo hóa đơn mới</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "Bạn muốn tạo hóa đơn mới không?"
+- Thêm thông tin đơn hàng thành công</t>
+  </si>
+  <si>
+    <t>SCM-23</t>
+  </si>
+  <si>
+    <t>SCM-25</t>
+  </si>
+  <si>
+    <t>SCM-26</t>
+  </si>
+  <si>
+    <t>Sửa thông tin đơn hàng(Sửa thông tin nhân viên, khách hàng, sản phẩm)</t>
+  </si>
+  <si>
+    <t>1. Chọn đơn hàng bất kỳ trong danh sách đơn hàng.
+2. Chọn lại thông tin nhân viên/khách hàng/sản phẩm.
+3. Bấm nút "Sửa"</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "Bạn có muốn sửa hóa đơn được chọn không".
+- Hóa đơn được sửa thành công</t>
+  </si>
+  <si>
+    <t>SCM-24</t>
+  </si>
+  <si>
+    <t>Sửa thông tin đơn hàng(Xóa trống trường dữ liệu số lượng hoặc giảm giá)</t>
+  </si>
+  <si>
+    <t>1. Chọn đơn hàng bất kỳ trong danh sách đơn hàng.
+2. Xóa trống dữ liệu ô Số lượng hoặc Giảm giá.
+3. Bấm nút "Sửa"</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "Không thể sửa - dữ liệu không hợp lệ"
+- Sửa dữ liệu thất bại</t>
+  </si>
+  <si>
+    <t>SCM-27</t>
+  </si>
+  <si>
+    <t>- Sản phẩm cần tìm hiển thị trong danh sách phía dưới
+- Tìm kiếm thông tin sản phẩm được nhập thành công</t>
+  </si>
+  <si>
+    <t>Tìm kiếm danh mục sản phẩm (Tìm theo tên sản phẩm - Nhập đúng tên)</t>
+  </si>
+  <si>
+    <t>Tìm kiếm danh mục sản phẩm (Tìm theo tên sản phẩm - Nhập sai tên)</t>
+  </si>
+  <si>
+    <t>- Sản phẩm cần tìm không được hiển thị.
+- Tìm kiếm thất bại</t>
+  </si>
+  <si>
+    <t>Tìm kiếm danh mục sản phẩm (Tìm theo mã sản phẩm - Nhập đúng mã)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click vào ô tìm kiếm 
+2. Click vào nút "Theo tên"
+3. Nhập </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sai</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> tên sản phẩm 
+4. Bấm vào button "Tìm kiếm"</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Click vào ô tìm kiếm 
+2. Click vào nút "Theo tên"
+3. Nhập đúng tên sản phẩm 
+4. Bấm vào button "Tìm kiếm"</t>
+  </si>
+  <si>
+    <t>1. Click vào ô tìm kiếm 
+2. Click vào nút "Theo mã"
+3. Nhập số 2
+4. Bấm vào button "Tìm kiếm"</t>
+  </si>
+  <si>
+    <t>- Sản phẩm cần tìm là Gạch Phước Thành được hiển thị
+- Tìm kiếm thành công</t>
+  </si>
+  <si>
+    <t>Tìm kiếm danh mục sản phẩm (Tìm theo mã sản phẩm - Nhập số - mã sai)</t>
+  </si>
+  <si>
+    <t>1. Click vào ô tìm kiếm 
+2. Click vào nút "Theo mã"
+3. Nhập số 1000
+4. Bấm vào button "Tìm kiếm"</t>
+  </si>
+  <si>
+    <t>SCM-28</t>
+  </si>
+  <si>
+    <t>SCM-29</t>
+  </si>
+  <si>
+    <t>Tìm kiếm danh mục sản phẩm (Tìm theo mã sản phẩm - Nhập vào là chữ cái)</t>
+  </si>
+  <si>
+    <t>1. Click vào ô tìm kiếm 
+2. Click vào nút "Theo mã"
+3. Nhập chữ abc
+4. Bấm vào button "Tìm kiếm"</t>
+  </si>
+  <si>
+    <t>SCM-30</t>
+  </si>
+  <si>
+    <t>Tìm kiếm đơn hàng (Tìm theo mã khách hàng - Nhập vào là chữ cái)</t>
+  </si>
+  <si>
+    <t>1. Click vào ô tìm kiếm 
+2. Click vào nút "Theo mã khách hàng"
+3. Nhập chữ abc
+4. Bấm vào button "Tìm kiếm"</t>
+  </si>
+  <si>
+    <t>SCM-31</t>
+  </si>
+  <si>
+    <t>Tìm kiếm đơn hàng (Tìm theo mã khách hàng - Nhập đúng mã khách hàng)</t>
+  </si>
+  <si>
+    <t>1. Click vào ô tìm kiếm 
+2. Click vào nút "Theo mã khách hàng"
+3. Nhập 8
+4. Bấm vào button "Tìm kiếm"</t>
+  </si>
+  <si>
+    <t>- Đơn hàng có mã 4008 được hiển thị
+- Tìm kiếm thành công</t>
+  </si>
+  <si>
+    <t>Tìm kiếm đơn hàng (Tìm theo mã đơn hàng - Nhập đúng mã đơn hàng)</t>
+  </si>
+  <si>
+    <t>1. Click vào ô tìm kiếm 
+2. Click vào nút "Theo mã đơn hàng"
+3. Nhập 4008
+4. Bấm vào button "Tìm kiếm"</t>
+  </si>
+  <si>
+    <t>- Đơn hàng có mã 4008 và mã Khách hàng là 8 được hiển thị
+- Tìm kiếm thành công</t>
+  </si>
+  <si>
+    <t>SCM-32</t>
+  </si>
+  <si>
+    <t>SCM-33</t>
+  </si>
+  <si>
+    <t>Tìm kiếm đơn hàng (Tìm theo mã đơn hàng - Nhập sai mã đơn hàng)</t>
+  </si>
+  <si>
+    <t>1. Click vào ô tìm kiếm 
+2. Click vào nút "Theo mã đơn hàng"
+3. Nhập 10000
+4. Bấm vào button "Tìm kiếm"</t>
+  </si>
+  <si>
+    <t>SCM-34</t>
+  </si>
+  <si>
+    <t>Tìm kiếm đơn hàng (Tìm theo mã đơn hàng - Nhập vào chữ cái)</t>
+  </si>
+  <si>
+    <t>1. Click vào ô tìm kiếm 
+2. Click vào nút "Theo mã đơn hàng"
+3. Nhập abc
+4. Bấm vào button "Tìm kiếm"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,6 +802,12 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -858,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -990,6 +1233,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1001,12 +1253,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1032,192 +1278,1074 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="95">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+  <dxfs count="221">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2138,7 +3266,7 @@
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
-      <c r="E1" s="59"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -2147,47 +3275,47 @@
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="I2" s="53"/>
+      <c r="J2" s="54" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="54"/>
+      <c r="J3" s="55"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
@@ -2238,7 +3366,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="5"/>
@@ -2253,8 +3381,8 @@
       <c r="C8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="15"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -2267,8 +3395,8 @@
       <c r="C9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="15"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -2281,8 +3409,8 @@
       <c r="C10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59"/>
       <c r="F10" s="15"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -2314,11 +3442,11 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -2341,11 +3469,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="G2:G3"/>
@@ -2355,6 +3478,11 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -2365,8 +3493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2531,7 +3659,9 @@
         <v>47</v>
       </c>
       <c r="J5" s="20"/>
-      <c r="K5" s="24"/>
+      <c r="K5" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -2561,7 +3691,9 @@
         <v>51</v>
       </c>
       <c r="J6" s="20"/>
-      <c r="K6" s="24"/>
+      <c r="K6" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -2591,7 +3723,9 @@
         <v>55</v>
       </c>
       <c r="J7" s="20"/>
-      <c r="K7" s="24"/>
+      <c r="K7" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -2621,7 +3755,9 @@
         <v>59</v>
       </c>
       <c r="J8" s="19"/>
-      <c r="K8" s="24"/>
+      <c r="K8" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -2653,7 +3789,9 @@
         <v>66</v>
       </c>
       <c r="J9" s="19"/>
-      <c r="K9" s="24"/>
+      <c r="K9" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L9" s="19"/>
     </row>
     <row r="10" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -2685,7 +3823,9 @@
         <v>76</v>
       </c>
       <c r="J10" s="19"/>
-      <c r="K10" s="24"/>
+      <c r="K10" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -2716,8 +3856,12 @@
       <c r="I11" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="24"/>
+      <c r="J11" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -2748,8 +3892,12 @@
       <c r="I12" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="24"/>
+      <c r="J12" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:22" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2781,7 +3929,9 @@
         <v>85</v>
       </c>
       <c r="J13" s="19"/>
-      <c r="K13" s="24"/>
+      <c r="K13" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L13" s="19"/>
     </row>
     <row r="14" spans="1:22" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2812,8 +3962,12 @@
       <c r="I14" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="24"/>
+      <c r="J14" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K14" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -2844,8 +3998,12 @@
       <c r="I15" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="24"/>
+      <c r="J15" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K15" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -2876,8 +4034,12 @@
       <c r="I16" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="24"/>
+      <c r="J16" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K16" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L16" s="19"/>
     </row>
     <row r="17" spans="1:12" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -2908,8 +4070,12 @@
       <c r="I17" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="24"/>
+      <c r="J17" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K17" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L17" s="19"/>
     </row>
     <row r="18" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2940,8 +4106,12 @@
       <c r="I18" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="24"/>
+      <c r="J18" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L18" s="19"/>
     </row>
     <row r="19" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2972,8 +4142,12 @@
       <c r="I19" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="24"/>
+      <c r="J19" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K19" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L19" s="19"/>
     </row>
     <row r="20" spans="1:12" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -3004,8 +4178,12 @@
       <c r="I20" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="24"/>
+      <c r="J20" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K20" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L20" s="19"/>
     </row>
     <row r="21" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -3036,248 +4214,532 @@
       <c r="I21" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="24"/>
+      <c r="J21" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K21" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L21" s="19"/>
     </row>
     <row r="22" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24">
         <v>20</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="B22" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="23">
+        <v>2</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>124</v>
+      </c>
       <c r="J22" s="19"/>
-      <c r="K22" s="24"/>
+      <c r="K22" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L22" s="19"/>
     </row>
     <row r="23" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24">
         <v>21</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="B23" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="23">
+        <v>2</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="28" t="s">
+        <v>124</v>
+      </c>
       <c r="J23" s="19"/>
-      <c r="K23" s="24"/>
+      <c r="K23" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L23" s="19"/>
     </row>
     <row r="24" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24">
         <v>22</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="B24" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="23">
+        <v>2</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>130</v>
+      </c>
       <c r="J24" s="19"/>
-      <c r="K24" s="24"/>
+      <c r="K24" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L24" s="19"/>
     </row>
-    <row r="25" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24">
         <v>23</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="B25" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="23">
+        <v>2</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>136</v>
+      </c>
       <c r="J25" s="19"/>
-      <c r="K25" s="24"/>
+      <c r="K25" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L25" s="19"/>
     </row>
-    <row r="26" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24">
         <v>24</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="24"/>
+      <c r="B26" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="23">
+        <v>2</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="J26" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K26" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L26" s="19"/>
     </row>
     <row r="27" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24">
         <v>25</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
+      <c r="B27" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E27" s="23">
+        <v>3</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>142</v>
+      </c>
       <c r="J27" s="19"/>
-      <c r="K27" s="24"/>
+      <c r="K27" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L27" s="19"/>
     </row>
     <row r="28" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24">
         <v>26</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
+      <c r="B28" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" s="23">
+        <v>3</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>145</v>
+      </c>
       <c r="J28" s="19"/>
-      <c r="K28" s="24"/>
+      <c r="K28" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L28" s="19"/>
     </row>
     <row r="29" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24">
         <v>27</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
+      <c r="B29" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="23">
+        <v>3</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>150</v>
+      </c>
       <c r="J29" s="19"/>
-      <c r="K29" s="24"/>
+      <c r="K29" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L29" s="19"/>
     </row>
     <row r="30" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24">
         <v>28</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
+      <c r="B30" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="23">
+        <v>3</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>145</v>
+      </c>
       <c r="J30" s="19"/>
-      <c r="K30" s="24"/>
+      <c r="K30" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L30" s="19"/>
     </row>
     <row r="31" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24">
         <v>29</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="24"/>
+      <c r="B31" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E31" s="23">
+        <v>3</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="I31" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="J31" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K31" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L31" s="19"/>
     </row>
-    <row r="32" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24">
         <v>30</v>
       </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="24"/>
+      <c r="B32" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" s="23">
+        <v>3</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="J32" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K32" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L32" s="19"/>
     </row>
-    <row r="33" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24">
         <v>31</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="24"/>
+      <c r="B33" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" s="23">
+        <v>3</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="J33" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K33" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L33" s="19"/>
     </row>
-    <row r="34" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24">
         <v>32</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
+      <c r="B34" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E34" s="23">
+        <v>3</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="I34" s="28" t="s">
+        <v>166</v>
+      </c>
       <c r="J34" s="19"/>
-      <c r="K34" s="24"/>
+      <c r="K34" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L34" s="19"/>
     </row>
     <row r="35" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24">
         <v>33</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
+      <c r="B35" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="E35" s="23">
+        <v>3</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="I35" s="28" t="s">
+        <v>145</v>
+      </c>
       <c r="J35" s="19"/>
-      <c r="K35" s="24"/>
+      <c r="K35" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L35" s="19"/>
     </row>
-    <row r="36" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24">
         <v>34</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="24"/>
+      <c r="B36" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="23">
+        <v>3</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="I36" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="J36" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K36" s="34" t="s">
+        <v>120</v>
+      </c>
       <c r="L36" s="19"/>
     </row>
     <row r="37" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -4133,329 +5595,646 @@
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K1:K2 K19:K20 K5:K17">
-    <cfRule type="containsText" dxfId="94" priority="90" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K1:K2">
+    <cfRule type="containsText" dxfId="220" priority="183" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5:K17 K19:K20">
-    <cfRule type="containsText" dxfId="93" priority="88" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K22">
+    <cfRule type="containsText" dxfId="214" priority="174" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="containsText" dxfId="213" priority="172" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="212" priority="173" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K26">
+    <cfRule type="containsText" dxfId="211" priority="171" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K26">
+    <cfRule type="containsText" dxfId="210" priority="169" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="209" priority="170" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K37:K45">
+    <cfRule type="containsText" dxfId="199" priority="159" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K37:K45">
+    <cfRule type="containsText" dxfId="198" priority="157" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="197" priority="158" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46">
+    <cfRule type="containsText" dxfId="196" priority="156" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46">
+    <cfRule type="containsText" dxfId="195" priority="154" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="194" priority="155" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="containsText" dxfId="193" priority="153" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="containsText" dxfId="192" priority="151" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="191" priority="152" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="containsText" dxfId="190" priority="150" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="containsText" dxfId="189" priority="148" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="188" priority="149" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K55">
+    <cfRule type="containsText" dxfId="187" priority="147" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K55">
+    <cfRule type="containsText" dxfId="186" priority="145" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="185" priority="146" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:K61">
+    <cfRule type="containsText" dxfId="184" priority="132" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:K61">
+    <cfRule type="containsText" dxfId="183" priority="130" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="182" priority="131" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="containsText" dxfId="181" priority="129" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="containsText" dxfId="180" priority="127" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="179" priority="128" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="containsText" dxfId="178" priority="126" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="containsText" dxfId="177" priority="124" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="176" priority="125" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="175" priority="123" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="174" priority="121" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="173" priority="122" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65:K71">
+    <cfRule type="containsText" dxfId="172" priority="120" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65:K71">
+    <cfRule type="containsText" dxfId="171" priority="118" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="170" priority="119" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:K79">
+    <cfRule type="containsText" dxfId="169" priority="117" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:K79">
+    <cfRule type="containsText" dxfId="168" priority="115" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K72)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="167" priority="116" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80">
+    <cfRule type="containsText" dxfId="166" priority="114" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80">
+    <cfRule type="containsText" dxfId="165" priority="112" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K80)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="164" priority="113" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81">
+    <cfRule type="containsText" dxfId="163" priority="111" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81">
+    <cfRule type="containsText" dxfId="162" priority="109" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K81)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="161" priority="110" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82">
+    <cfRule type="containsText" dxfId="160" priority="108" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82">
+    <cfRule type="containsText" dxfId="159" priority="106" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K82)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="158" priority="107" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K83:K89">
+    <cfRule type="containsText" dxfId="157" priority="105" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K83:K89">
+    <cfRule type="containsText" dxfId="156" priority="103" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K83)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="155" priority="104" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="151" priority="99" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="150" priority="97" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="149" priority="98" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="containsText" dxfId="148" priority="96" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="containsText" dxfId="147" priority="94" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="146" priority="95" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="containsText" dxfId="128" priority="93" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="containsText" dxfId="127" priority="91" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="89" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="126" priority="92" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K5)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="containsText" dxfId="125" priority="90" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="containsText" dxfId="124" priority="88" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="123" priority="89" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="containsText" dxfId="122" priority="87" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="containsText" dxfId="121" priority="85" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="86" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="containsText" dxfId="119" priority="84" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="containsText" dxfId="118" priority="82" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="83" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="containsText" dxfId="116" priority="81" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="containsText" dxfId="115" priority="79" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="80" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="containsText" dxfId="113" priority="78" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="containsText" dxfId="112" priority="76" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="111" priority="77" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="containsText" dxfId="110" priority="75" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="containsText" dxfId="109" priority="73" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="74" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="containsText" dxfId="107" priority="72" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="containsText" dxfId="106" priority="70" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="71" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="containsText" dxfId="104" priority="69" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="containsText" dxfId="103" priority="67" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="68" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="containsText" dxfId="101" priority="66" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="containsText" dxfId="100" priority="64" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="65" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="containsText" dxfId="98" priority="63" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="containsText" dxfId="97" priority="61" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="96" priority="62" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="containsText" dxfId="95" priority="60" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="containsText" dxfId="94" priority="58" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="93" priority="59" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsText" dxfId="92" priority="57" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsText" dxfId="91" priority="55" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="56" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="89" priority="54" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="88" priority="52" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="87" priority="53" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="containsText" dxfId="86" priority="51" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="containsText" dxfId="85" priority="49" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="84" priority="50" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20">
+    <cfRule type="containsText" dxfId="83" priority="48" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20">
+    <cfRule type="containsText" dxfId="82" priority="46" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="81" priority="47" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="91" priority="84" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="80" priority="45" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="90" priority="82" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="79" priority="43" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="83" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="78" priority="44" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
-    <cfRule type="containsText" dxfId="88" priority="81" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
-    <cfRule type="containsText" dxfId="87" priority="79" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="80" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23:K29">
-    <cfRule type="containsText" dxfId="85" priority="78" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K23">
+    <cfRule type="containsText" dxfId="77" priority="42" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K23)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K23:K29">
-    <cfRule type="containsText" dxfId="84" priority="76" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K23">
+    <cfRule type="containsText" dxfId="76" priority="40" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="77" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="75" priority="41" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K23)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K24">
+    <cfRule type="containsText" dxfId="74" priority="39" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24">
+    <cfRule type="containsText" dxfId="73" priority="37" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="38" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
+    <cfRule type="containsText" dxfId="65" priority="33" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
+    <cfRule type="containsText" dxfId="63" priority="31" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="32" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27">
+    <cfRule type="containsText" dxfId="59" priority="30" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27">
+    <cfRule type="containsText" dxfId="57" priority="28" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="29" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28">
+    <cfRule type="containsText" dxfId="53" priority="27" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28">
+    <cfRule type="containsText" dxfId="51" priority="25" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="26" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29">
+    <cfRule type="containsText" dxfId="47" priority="24" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29">
+    <cfRule type="containsText" dxfId="45" priority="22" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="23" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="82" priority="75" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="41" priority="21" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="81" priority="73" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="39" priority="19" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="74" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="38" priority="20" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="79" priority="72" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="35" priority="18" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="78" priority="70" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="33" priority="16" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="71" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="32" priority="17" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="76" priority="69" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="75" priority="67" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="27" priority="13" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="68" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="26" priority="14" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33:K45">
-    <cfRule type="containsText" dxfId="73" priority="66" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K33">
+    <cfRule type="containsText" dxfId="23" priority="12" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33:K45">
-    <cfRule type="containsText" dxfId="72" priority="64" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K33">
+    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="65" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="20" priority="11" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="70" priority="63" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="69" priority="61" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="62" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47">
-    <cfRule type="containsText" dxfId="67" priority="60" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47">
-    <cfRule type="containsText" dxfId="66" priority="58" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="59" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K48">
-    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K48">
-    <cfRule type="containsText" dxfId="63" priority="55" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="56" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K49:K55">
-    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K49:K55">
-    <cfRule type="containsText" dxfId="60" priority="52" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K56:K61">
-    <cfRule type="containsText" dxfId="58" priority="39" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K56:K61">
-    <cfRule type="containsText" dxfId="57" priority="37" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="38" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="containsText" dxfId="54" priority="34" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K62)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="35" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="29" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65:K71">
-    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65:K71">
-    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72:K79">
-    <cfRule type="containsText" dxfId="43" priority="24" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72:K79">
-    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K72)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K80">
-    <cfRule type="containsText" dxfId="40" priority="21" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K80)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K80">
-    <cfRule type="containsText" dxfId="39" priority="19" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K80)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="20" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K80)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81">
-    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81">
-    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K81)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="17" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82">
-    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82">
-    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K82)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K83:K89">
-    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K83)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K83:K89">
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K83)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K83)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
+  <conditionalFormatting sqref="K34">
+    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K34">
+    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K35">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K35">
+    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36">
     <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Failed",K36)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Passed",K36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -4625,77 +6404,77 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="L1">
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="145" priority="20" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="144" priority="16" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="containsText" dxfId="23" priority="15" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="143" priority="15" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="containsText" dxfId="22" priority="13" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="142" priority="13" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="141" priority="14" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="containsText" dxfId="20" priority="12" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="140" priority="12" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="containsText" dxfId="19" priority="10" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="139" priority="10" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="138" priority="11" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="137" priority="9" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="containsText" dxfId="16" priority="7" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="136" priority="7" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="135" priority="8" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="134" priority="6" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="133" priority="4" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="132" priority="5" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="131" priority="3" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="130" priority="1" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="129" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L7)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Test Case Quan ly
</commit_message>
<xml_diff>
--- a/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
+++ b/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="188">
   <si>
     <t>1.    Phạm vi test</t>
   </si>
@@ -719,6 +719,59 @@
 2. Click vào nút "Theo mã đơn hàng"
 3. Nhập abc
 4. Bấm vào button "Tìm kiếm"</t>
+  </si>
+  <si>
+    <t>Quản lý</t>
+  </si>
+  <si>
+    <t>Đăng nhập (Không biết tài khoản đăng nhập vào hệ thống)</t>
+  </si>
+  <si>
+    <t>1. Click vào nút "Quản lý"
+2. Điền tên đăng nhập: abc
+3. Điền mật khẩu: 123456
+4. Bấm nút "Đăng nhập".</t>
+  </si>
+  <si>
+    <t>- Hiển thị hộp thoại thông báo "Bạn đã nhập sai tên đăng nhập và mật khẩu - Yêu cầu đăng nhập lại".
+- Không thể vào hệ thống quản lý, quay lại Form "Đăng nhập" vào quản lý.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SCM-35</t>
+  </si>
+  <si>
+    <t>SCM-36</t>
+  </si>
+  <si>
+    <t>Đăng nhập (Sử dụng tài khoản với quyền là Nhân viên)</t>
+  </si>
+  <si>
+    <t>1. Click vào nút "Quản lý"
+2. Điền tên đăng nhập: Huy
+3. Điền mật khẩu: 123
+4. Bấm nút "Đăng nhập".</t>
+  </si>
+  <si>
+    <t>- Hiển thị hộp thoại thông báo "Tài khoản này không có quyền vào quản lý - Yêu cầu đăng nhập lại".
+- Không thể vào hệ thống quản lý, quay lại Form "Đăng nhập" vào quản lý.</t>
+  </si>
+  <si>
+    <t>SCM-37</t>
+  </si>
+  <si>
+    <t>Đăng nhập (Sử dụng tài khoản với quyền là Quản lý)</t>
+  </si>
+  <si>
+    <t>1. Click vào nút "Quản lý"
+2. Điền tên đăng nhập: Long
+3. Điền mật khẩu: 123
+4. Bấm nút "Đăng nhập".</t>
+  </si>
+  <si>
+    <t>- Đăng nhập thành công vào form quản lý hệ thống</t>
   </si>
 </sst>
 </file>
@@ -1227,20 +1280,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1253,6 +1300,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1278,20 +1331,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="221">
+  <dxfs count="183">
     <dxf>
       <fill>
         <patternFill>
@@ -1435,6 +1488,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -1456,6 +1516,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1477,6 +1551,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -1505,6 +1586,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -1519,6 +1607,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -1540,6 +1635,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1561,6 +1670,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -1582,6 +1698,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1603,6 +1733,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -1624,6 +1761,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1645,6 +1796,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -1666,6 +1824,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1687,6 +1859,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -1708,6 +1887,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1729,6 +1922,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -1750,6 +1950,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1771,6 +1985,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -1792,6 +2013,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -2303,6 +2538,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -2310,6 +2559,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -2353,482 +2616,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3260,13 +3047,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -3275,22 +3062,22 @@
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="50" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="52" t="s">
@@ -3303,12 +3090,12 @@
     </row>
     <row r="3" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3362,11 +3149,11 @@
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="48"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="5"/>
@@ -3442,11 +3229,11 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -3469,6 +3256,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="G2:G3"/>
@@ -3478,11 +3270,6 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -3493,8 +3280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3514,20 +3301,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="30" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:22" s="21" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -3856,7 +3643,7 @@
       <c r="I11" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="62" t="s">
+      <c r="J11" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K11" s="34" t="s">
@@ -3892,7 +3679,7 @@
       <c r="I12" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="62" t="s">
+      <c r="J12" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K12" s="34" t="s">
@@ -3962,7 +3749,7 @@
       <c r="I14" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="62" t="s">
+      <c r="J14" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K14" s="34" t="s">
@@ -3998,7 +3785,7 @@
       <c r="I15" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="J15" s="62" t="s">
+      <c r="J15" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K15" s="34" t="s">
@@ -4034,7 +3821,7 @@
       <c r="I16" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J16" s="62" t="s">
+      <c r="J16" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K16" s="34" t="s">
@@ -4070,7 +3857,7 @@
       <c r="I17" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="J17" s="62" t="s">
+      <c r="J17" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K17" s="34" t="s">
@@ -4106,7 +3893,7 @@
       <c r="I18" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="J18" s="62" t="s">
+      <c r="J18" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K18" s="34" t="s">
@@ -4142,7 +3929,7 @@
       <c r="I19" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="J19" s="62" t="s">
+      <c r="J19" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K19" s="34" t="s">
@@ -4178,7 +3965,7 @@
       <c r="I20" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="J20" s="62" t="s">
+      <c r="J20" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K20" s="34" t="s">
@@ -4214,7 +4001,7 @@
       <c r="I21" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="J21" s="62" t="s">
+      <c r="J21" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K21" s="34" t="s">
@@ -4386,7 +4173,7 @@
       <c r="I26" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="J26" s="62" t="s">
+      <c r="J26" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K26" s="34" t="s">
@@ -4558,7 +4345,7 @@
       <c r="I31" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="J31" s="62" t="s">
+      <c r="J31" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K31" s="34" t="s">
@@ -4594,7 +4381,7 @@
       <c r="I32" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="J32" s="62" t="s">
+      <c r="J32" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K32" s="34" t="s">
@@ -4630,7 +4417,7 @@
       <c r="I33" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="J33" s="62" t="s">
+      <c r="J33" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K33" s="34" t="s">
@@ -4734,7 +4521,7 @@
       <c r="I36" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="J36" s="62" t="s">
+      <c r="J36" s="43" t="s">
         <v>121</v>
       </c>
       <c r="K36" s="34" t="s">
@@ -4746,48 +4533,104 @@
       <c r="A37" s="24">
         <v>35</v>
       </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="24"/>
+      <c r="B37" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" s="23">
+        <v>2</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="I37" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="K37" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L37" s="19"/>
     </row>
     <row r="38" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24">
         <v>36</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
+      <c r="B38" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="E38" s="23">
+        <v>2</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="I38" s="28" t="s">
+        <v>183</v>
+      </c>
       <c r="J38" s="19"/>
-      <c r="K38" s="24"/>
+      <c r="K38" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L38" s="19"/>
     </row>
     <row r="39" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24">
         <v>37</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
+      <c r="B39" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" s="23">
+        <v>2</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="I39" s="28" t="s">
+        <v>187</v>
+      </c>
       <c r="J39" s="19"/>
-      <c r="K39" s="24"/>
+      <c r="K39" s="34" t="s">
+        <v>116</v>
+      </c>
       <c r="L39" s="19"/>
     </row>
     <row r="40" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -5596,645 +5439,684 @@
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="K1:K2">
-    <cfRule type="containsText" dxfId="220" priority="183" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="182" priority="192" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="containsText" dxfId="214" priority="174" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="181" priority="183" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="containsText" dxfId="213" priority="172" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="180" priority="181" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="212" priority="173" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="179" priority="182" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="containsText" dxfId="211" priority="171" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="178" priority="180" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="containsText" dxfId="210" priority="169" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="177" priority="178" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="170" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="176" priority="179" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K26)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K37:K45">
-    <cfRule type="containsText" dxfId="199" priority="159" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K40:K45">
+    <cfRule type="containsText" dxfId="175" priority="168" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K40:K45">
+    <cfRule type="containsText" dxfId="174" priority="166" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="173" priority="167" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46">
+    <cfRule type="containsText" dxfId="172" priority="165" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46">
+    <cfRule type="containsText" dxfId="171" priority="163" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="170" priority="164" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="containsText" dxfId="169" priority="162" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="containsText" dxfId="168" priority="160" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="167" priority="161" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="containsText" dxfId="166" priority="159" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="containsText" dxfId="165" priority="157" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="164" priority="158" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K55">
+    <cfRule type="containsText" dxfId="163" priority="156" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K55">
+    <cfRule type="containsText" dxfId="162" priority="154" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="161" priority="155" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:K61">
+    <cfRule type="containsText" dxfId="160" priority="141" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:K61">
+    <cfRule type="containsText" dxfId="159" priority="139" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="158" priority="140" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="containsText" dxfId="157" priority="138" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="containsText" dxfId="156" priority="136" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="155" priority="137" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="containsText" dxfId="154" priority="135" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="containsText" dxfId="153" priority="133" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="152" priority="134" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="151" priority="132" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="150" priority="130" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="149" priority="131" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65:K71">
+    <cfRule type="containsText" dxfId="148" priority="129" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65:K71">
+    <cfRule type="containsText" dxfId="147" priority="127" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="146" priority="128" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:K79">
+    <cfRule type="containsText" dxfId="145" priority="126" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:K79">
+    <cfRule type="containsText" dxfId="144" priority="124" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K72)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="143" priority="125" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80">
+    <cfRule type="containsText" dxfId="142" priority="123" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80">
+    <cfRule type="containsText" dxfId="141" priority="121" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K80)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="140" priority="122" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81">
+    <cfRule type="containsText" dxfId="139" priority="120" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81">
+    <cfRule type="containsText" dxfId="138" priority="118" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K81)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="137" priority="119" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82">
+    <cfRule type="containsText" dxfId="136" priority="117" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82">
+    <cfRule type="containsText" dxfId="135" priority="115" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K82)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="134" priority="116" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K83:K89">
+    <cfRule type="containsText" dxfId="133" priority="114" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K83:K89">
+    <cfRule type="containsText" dxfId="132" priority="112" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K83)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="131" priority="113" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="130" priority="108" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="129" priority="106" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="128" priority="107" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="containsText" dxfId="127" priority="105" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="containsText" dxfId="126" priority="103" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="125" priority="104" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="containsText" dxfId="124" priority="102" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="containsText" dxfId="123" priority="100" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="122" priority="101" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="containsText" dxfId="121" priority="99" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="containsText" dxfId="120" priority="97" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="119" priority="98" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="containsText" dxfId="118" priority="96" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="containsText" dxfId="117" priority="94" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="116" priority="95" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="containsText" dxfId="115" priority="93" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="containsText" dxfId="114" priority="91" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="113" priority="92" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="containsText" dxfId="112" priority="90" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="containsText" dxfId="111" priority="88" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="110" priority="89" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="containsText" dxfId="109" priority="87" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="containsText" dxfId="108" priority="85" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="107" priority="86" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="containsText" dxfId="106" priority="84" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="containsText" dxfId="105" priority="82" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="104" priority="83" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="containsText" dxfId="103" priority="81" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="containsText" dxfId="102" priority="79" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="101" priority="80" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="containsText" dxfId="100" priority="78" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="containsText" dxfId="99" priority="76" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="98" priority="77" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="containsText" dxfId="97" priority="75" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="containsText" dxfId="96" priority="73" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="95" priority="74" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="containsText" dxfId="94" priority="72" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="containsText" dxfId="93" priority="70" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="containsText" dxfId="91" priority="69" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="containsText" dxfId="90" priority="67" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="68" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsText" dxfId="88" priority="66" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsText" dxfId="87" priority="64" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="86" priority="65" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="85" priority="63" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="84" priority="61" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="83" priority="62" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="containsText" dxfId="82" priority="60" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="containsText" dxfId="81" priority="58" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="59" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20">
+    <cfRule type="containsText" dxfId="79" priority="57" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20">
+    <cfRule type="containsText" dxfId="78" priority="55" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="56" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="containsText" dxfId="76" priority="54" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="containsText" dxfId="75" priority="52" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="53" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="containsText" dxfId="73" priority="51" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="containsText" dxfId="72" priority="49" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="71" priority="50" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24">
+    <cfRule type="containsText" dxfId="70" priority="48" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24">
+    <cfRule type="containsText" dxfId="69" priority="46" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="47" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
+    <cfRule type="containsText" dxfId="67" priority="42" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
+    <cfRule type="containsText" dxfId="66" priority="40" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="41" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27">
+    <cfRule type="containsText" dxfId="64" priority="39" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27">
+    <cfRule type="containsText" dxfId="63" priority="37" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="38" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28">
+    <cfRule type="containsText" dxfId="61" priority="36" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28">
+    <cfRule type="containsText" dxfId="60" priority="34" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="35" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29">
+    <cfRule type="containsText" dxfId="58" priority="33" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29">
+    <cfRule type="containsText" dxfId="57" priority="31" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="32" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30">
+    <cfRule type="containsText" dxfId="55" priority="30" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30">
+    <cfRule type="containsText" dxfId="54" priority="28" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="29" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="containsText" dxfId="52" priority="27" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="containsText" dxfId="51" priority="25" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="26" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32">
+    <cfRule type="containsText" dxfId="49" priority="24" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32">
+    <cfRule type="containsText" dxfId="48" priority="22" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="23" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33">
+    <cfRule type="containsText" dxfId="46" priority="21" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33">
+    <cfRule type="containsText" dxfId="45" priority="19" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="20" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K34">
+    <cfRule type="containsText" dxfId="43" priority="18" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K34">
+    <cfRule type="containsText" dxfId="42" priority="16" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="17" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K35">
+    <cfRule type="containsText" dxfId="40" priority="15" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K35">
+    <cfRule type="containsText" dxfId="39" priority="13" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="14" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36">
+    <cfRule type="containsText" dxfId="37" priority="12" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36">
+    <cfRule type="containsText" dxfId="36" priority="10" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="11" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K37">
+    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K37)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K37:K45">
-    <cfRule type="containsText" dxfId="198" priority="157" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K37">
+    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="158" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K37)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="196" priority="156" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="195" priority="154" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="155" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47">
-    <cfRule type="containsText" dxfId="193" priority="153" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47">
-    <cfRule type="containsText" dxfId="192" priority="151" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="152" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K48">
-    <cfRule type="containsText" dxfId="190" priority="150" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K48">
-    <cfRule type="containsText" dxfId="189" priority="148" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="188" priority="149" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K49:K55">
-    <cfRule type="containsText" dxfId="187" priority="147" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K49:K55">
-    <cfRule type="containsText" dxfId="186" priority="145" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="146" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K56:K61">
-    <cfRule type="containsText" dxfId="184" priority="132" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K56:K61">
-    <cfRule type="containsText" dxfId="183" priority="130" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="131" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="containsText" dxfId="181" priority="129" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="containsText" dxfId="180" priority="127" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K62)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="179" priority="128" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="containsText" dxfId="178" priority="126" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="containsText" dxfId="177" priority="124" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="176" priority="125" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="175" priority="123" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="174" priority="121" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="122" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65:K71">
-    <cfRule type="containsText" dxfId="172" priority="120" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65:K71">
-    <cfRule type="containsText" dxfId="171" priority="118" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="119" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72:K79">
-    <cfRule type="containsText" dxfId="169" priority="117" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72:K79">
-    <cfRule type="containsText" dxfId="168" priority="115" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K72)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="116" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K80">
-    <cfRule type="containsText" dxfId="166" priority="114" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K80)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K80">
-    <cfRule type="containsText" dxfId="165" priority="112" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K80)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="113" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K80)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81">
-    <cfRule type="containsText" dxfId="163" priority="111" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81">
-    <cfRule type="containsText" dxfId="162" priority="109" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K81)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="110" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82">
-    <cfRule type="containsText" dxfId="160" priority="108" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82">
-    <cfRule type="containsText" dxfId="159" priority="106" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K82)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="107" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K83:K89">
-    <cfRule type="containsText" dxfId="157" priority="105" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K83)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K83:K89">
-    <cfRule type="containsText" dxfId="156" priority="103" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K83)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="155" priority="104" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K83)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3">
-    <cfRule type="containsText" dxfId="151" priority="99" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3">
-    <cfRule type="containsText" dxfId="150" priority="97" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="98" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
-    <cfRule type="containsText" dxfId="148" priority="96" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
-    <cfRule type="containsText" dxfId="147" priority="94" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="95" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
-    <cfRule type="containsText" dxfId="128" priority="93" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
-    <cfRule type="containsText" dxfId="127" priority="91" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="92" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="125" priority="90" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="124" priority="88" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="89" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="122" priority="87" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="121" priority="85" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="86" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K8">
-    <cfRule type="containsText" dxfId="119" priority="84" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K8">
-    <cfRule type="containsText" dxfId="118" priority="82" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="83" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="116" priority="81" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="115" priority="79" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="80" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="containsText" dxfId="113" priority="78" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="containsText" dxfId="112" priority="76" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="77" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11">
-    <cfRule type="containsText" dxfId="110" priority="75" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11">
-    <cfRule type="containsText" dxfId="109" priority="73" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="74" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="107" priority="72" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="106" priority="70" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="71" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
-    <cfRule type="containsText" dxfId="104" priority="69" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
-    <cfRule type="containsText" dxfId="103" priority="67" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="68" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="101" priority="66" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="100" priority="64" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="65" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="98" priority="63" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="97" priority="61" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="62" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="containsText" dxfId="95" priority="60" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="containsText" dxfId="94" priority="58" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="59" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="92" priority="57" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="91" priority="55" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="56" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="89" priority="54" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="88" priority="52" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="53" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19">
-    <cfRule type="containsText" dxfId="86" priority="51" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19">
-    <cfRule type="containsText" dxfId="85" priority="49" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="50" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="83" priority="48" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="82" priority="46" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="47" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="80" priority="45" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="79" priority="43" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="44" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
-    <cfRule type="containsText" dxfId="77" priority="42" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
-    <cfRule type="containsText" dxfId="76" priority="40" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="41" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
-    <cfRule type="containsText" dxfId="74" priority="39" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
-    <cfRule type="containsText" dxfId="73" priority="37" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="38" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
-    <cfRule type="containsText" dxfId="65" priority="33" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
-    <cfRule type="containsText" dxfId="63" priority="31" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="32" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
-    <cfRule type="containsText" dxfId="59" priority="30" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
-    <cfRule type="containsText" dxfId="57" priority="28" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="29" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
-    <cfRule type="containsText" dxfId="53" priority="27" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
-    <cfRule type="containsText" dxfId="51" priority="25" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="26" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
-    <cfRule type="containsText" dxfId="47" priority="24" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
-    <cfRule type="containsText" dxfId="45" priority="22" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="23" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="41" priority="21" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="39" priority="19" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="20" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="35" priority="18" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="33" priority="16" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="17" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="27" priority="13" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="14" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
-    <cfRule type="containsText" dxfId="23" priority="12" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
-    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K34">
-    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K34">
-    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K35">
+  <conditionalFormatting sqref="K38">
     <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K35">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K38">
     <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Failed",K38)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
+      <formula>NOT(ISERROR(SEARCH("Passed",K38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K39">
     <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K39">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K36)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Failed",K39)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K36)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Passed",K39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -6282,17 +6164,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="36" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
       <c r="L1" s="35"/>
@@ -6404,77 +6286,77 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="L1">
-    <cfRule type="containsText" dxfId="145" priority="20" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="34" priority="20" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="containsText" dxfId="144" priority="16" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="33" priority="16" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="containsText" dxfId="143" priority="15" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="32" priority="15" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="containsText" dxfId="142" priority="13" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="14" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="30" priority="14" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="containsText" dxfId="140" priority="12" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="29" priority="12" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="containsText" dxfId="139" priority="10" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="11" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="containsText" dxfId="137" priority="9" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="26" priority="9" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="containsText" dxfId="136" priority="7" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="25" priority="7" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="8" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="24" priority="8" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="containsText" dxfId="134" priority="6" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="23" priority="6" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="containsText" dxfId="133" priority="4" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="5" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="containsText" dxfId="131" priority="3" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="containsText" dxfId="130" priority="1" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L7)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>